<commit_message>
2410. Maximum Matching of Players With Trainers (two pointers , greedy ,sorting)
</commit_message>
<xml_diff>
--- a/50  days challenge/DSA_trackerSheet.xlsx
+++ b/50  days challenge/DSA_trackerSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="150">
   <si>
     <t>Q No.</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>String ,Two Pointers , hashmap</t>
+  </si>
+  <si>
+    <t>Maximum Matching of Players With Trainers</t>
+  </si>
+  <si>
+    <t>Two Pointer, Sorting , Greedy</t>
   </si>
   <si>
     <t>Sliding Window (Basics)</t>
@@ -708,7 +714,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,6 +736,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,7 +1106,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1118,16 +1130,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1136,89 +1148,89 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1243,6 +1255,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1252,7 +1270,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1270,28 +1288,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1834,10 +1852,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1878,7 +1896,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="13"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -1893,7 +1911,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="15">
         <v>45688</v>
       </c>
       <c r="F5" t="s">
@@ -1913,7 +1931,7 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="16">
         <v>45688</v>
       </c>
       <c r="F6" t="s">
@@ -1933,7 +1951,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="16">
         <v>45689</v>
       </c>
       <c r="F7" t="s">
@@ -1953,7 +1971,7 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="16">
         <v>45689</v>
       </c>
       <c r="F8" t="s">
@@ -1973,7 +1991,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="16">
         <v>45690</v>
       </c>
       <c r="F9" t="s">
@@ -1993,7 +2011,7 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="16">
         <v>45691</v>
       </c>
       <c r="F10" t="s">
@@ -2013,7 +2031,7 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="16">
         <v>45692</v>
       </c>
       <c r="F11" t="s">
@@ -2033,7 +2051,7 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="16">
         <v>45693</v>
       </c>
       <c r="F12" t="s">
@@ -2058,7 +2076,7 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="16">
         <v>45691</v>
       </c>
       <c r="F16" t="s">
@@ -2078,7 +2096,7 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="16">
         <v>45692</v>
       </c>
       <c r="F17" t="s">
@@ -2098,7 +2116,7 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="16">
         <v>45694</v>
       </c>
       <c r="F18" t="s">
@@ -2118,7 +2136,7 @@
       <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="16">
         <v>45697</v>
       </c>
       <c r="F19" t="s">
@@ -2138,7 +2156,7 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="16">
         <v>45700</v>
       </c>
       <c r="F20" t="s">
@@ -2158,7 +2176,7 @@
       <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="16">
         <v>45808</v>
       </c>
       <c r="F21" t="s">
@@ -2183,7 +2201,7 @@
       <c r="D25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="16">
         <v>45693</v>
       </c>
       <c r="F25" t="s">
@@ -2203,7 +2221,7 @@
       <c r="D26" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="16">
         <v>45694</v>
       </c>
       <c r="F26" t="s">
@@ -2223,7 +2241,7 @@
       <c r="D27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="16">
         <v>45826</v>
       </c>
       <c r="F27" t="s">
@@ -2243,7 +2261,7 @@
       <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="16">
         <v>45827</v>
       </c>
       <c r="F28" t="s">
@@ -2268,7 +2286,7 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="16">
         <v>45695</v>
       </c>
       <c r="F32" t="s">
@@ -2288,7 +2306,7 @@
       <c r="D33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="16">
         <v>45699</v>
       </c>
       <c r="F33" t="s">
@@ -2308,44 +2326,44 @@
       <c r="D34" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="16">
         <v>45746</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" ht="32" customHeight="1" spans="2:2">
-      <c r="B36" s="4" t="s">
+    <row r="35" ht="17" spans="1:6">
+      <c r="A35" s="8">
+        <v>2410</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>3</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="C38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E35" s="16">
+        <v>45851</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" ht="32" customHeight="1" spans="2:2">
+      <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="14">
-        <v>45700</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>567</v>
+        <v>3</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>54</v>
@@ -2356,18 +2374,18 @@
       <c r="D39" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="14">
-        <v>45701</v>
+      <c r="E39" s="16">
+        <v>45700</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" ht="18" spans="1:6">
+    <row r="40" spans="1:6">
       <c r="A40">
-        <v>2966</v>
-      </c>
-      <c r="B40" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C40" t="s">
@@ -2376,67 +2394,67 @@
       <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="14">
-        <v>45826</v>
+      <c r="E40" s="16">
+        <v>45701</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" ht="18" spans="1:6">
       <c r="A41">
-        <v>594</v>
-      </c>
-      <c r="B41" s="9" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="16">
+        <v>45826</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>594</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="16">
         <v>45838</v>
       </c>
-      <c r="F41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="9"/>
-      <c r="E42" s="14"/>
-    </row>
-    <row r="43" ht="39" customHeight="1" spans="2:2">
-      <c r="B43" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" ht="17" spans="1:6">
-      <c r="A45">
+      <c r="F42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="11"/>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" ht="39" customHeight="1" spans="2:2">
+      <c r="B44" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" ht="17" spans="1:6">
+      <c r="A46">
         <v>424</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" t="s">
-        <v>62</v>
-      </c>
-      <c r="E45" s="14">
-        <v>45716</v>
-      </c>
-      <c r="F45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46">
-        <v>2799</v>
-      </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C46" t="s">
@@ -2445,8 +2463,8 @@
       <c r="D46" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="14">
-        <v>45771</v>
+      <c r="E46" s="16">
+        <v>45716</v>
       </c>
       <c r="F46" t="s">
         <v>10</v>
@@ -2454,7 +2472,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>2962</v>
+        <v>2799</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>65</v>
@@ -2465,8 +2483,8 @@
       <c r="D47" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="14">
-        <v>45776</v>
+      <c r="E47" s="16">
+        <v>45771</v>
       </c>
       <c r="F47" t="s">
         <v>10</v>
@@ -2474,7 +2492,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>3439</v>
+        <v>2962</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>67</v>
@@ -2483,205 +2501,205 @@
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
-      </c>
-      <c r="E48" s="14">
+        <v>68</v>
+      </c>
+      <c r="E48" s="16">
+        <v>45776</v>
+      </c>
+      <c r="F48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>3439</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="16">
         <v>45847</v>
       </c>
-      <c r="F48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" ht="31" customHeight="1" spans="2:2">
-      <c r="B50" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
-        <v>3066</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" ht="31" customHeight="1" spans="2:2">
+      <c r="B51" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="E52" s="14">
-        <v>45701</v>
-      </c>
-      <c r="F52" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>2099</v>
+        <v>3066</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
         <v>72</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="16">
+        <v>45701</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>2099</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="16">
         <v>45836</v>
       </c>
-      <c r="F53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" ht="38" customHeight="1" spans="2:2">
-      <c r="B55" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
-        <v>20</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" ht="38" customHeight="1" spans="2:2">
+      <c r="B56" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="E57" s="14">
-        <v>45719</v>
-      </c>
-      <c r="F57" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
         <v>77</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E58" s="16">
+        <v>45719</v>
+      </c>
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>155</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" t="s">
+        <v>79</v>
+      </c>
+      <c r="E59" s="16">
         <v>45731</v>
       </c>
-      <c r="F58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" ht="40" customHeight="1" spans="2:2">
-      <c r="B60" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62">
+      <c r="F59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" ht="40" customHeight="1" spans="2:2">
+      <c r="B61" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
         <v>739</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" t="s">
-        <v>80</v>
-      </c>
-      <c r="E62" s="14">
-        <v>45732</v>
-      </c>
-      <c r="F62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" s="1" customFormat="1" spans="1:6">
-      <c r="A63" s="12">
-        <v>84</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E63" s="15">
+      <c r="E63" s="16">
+        <v>45732</v>
+      </c>
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" s="1" customFormat="1" spans="1:6">
+      <c r="A64" s="14">
+        <v>84</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E64" s="17">
         <v>45745</v>
       </c>
-      <c r="F63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" ht="34" customHeight="1" spans="2:2">
-      <c r="B65" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="67" ht="18" spans="1:6">
-      <c r="A67">
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" ht="34" customHeight="1" spans="2:2">
+      <c r="B66" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" ht="18" spans="1:6">
+      <c r="A68">
         <v>225</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B68" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" t="s">
         <v>8</v>
       </c>
-      <c r="D67" t="s">
-        <v>85</v>
-      </c>
-      <c r="E67" s="14">
+      <c r="D68" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68" s="16">
         <v>45841</v>
       </c>
-      <c r="F67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B69" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="71" customFormat="1" ht="18" spans="1:6">
-      <c r="A71">
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B70" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" ht="18" spans="1:6">
+      <c r="A72">
         <v>206</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" t="s">
-        <v>88</v>
-      </c>
-      <c r="E71" s="14">
-        <v>45746</v>
-      </c>
-      <c r="F71" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" customFormat="1" spans="1:6">
-      <c r="A72">
-        <v>21</v>
-      </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="10" t="s">
         <v>89</v>
       </c>
       <c r="C72" t="s">
@@ -2690,93 +2708,93 @@
       <c r="D72" t="s">
         <v>90</v>
       </c>
-      <c r="E72" s="14">
+      <c r="E72" s="16">
+        <v>45746</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" spans="1:6">
+      <c r="A73">
+        <v>21</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73" s="16">
         <v>45747</v>
       </c>
-      <c r="F72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" customFormat="1" spans="5:5">
-      <c r="E73" s="14"/>
-    </row>
-    <row r="74" customFormat="1" ht="26" customHeight="1" spans="2:5">
-      <c r="B74" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="14"/>
-    </row>
-    <row r="75" customFormat="1" spans="5:5">
-      <c r="E75" s="14"/>
-    </row>
-    <row r="76" customFormat="1" spans="1:6">
-      <c r="A76">
-        <v>2</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C76" t="s">
-        <v>24</v>
-      </c>
-      <c r="D76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" s="14">
-        <v>45747</v>
-      </c>
-      <c r="F76" t="s">
-        <v>10</v>
-      </c>
+      <c r="F73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" spans="5:5">
+      <c r="E74" s="16"/>
+    </row>
+    <row r="75" customFormat="1" ht="26" customHeight="1" spans="2:5">
+      <c r="B75" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" s="16"/>
+    </row>
+    <row r="76" customFormat="1" spans="5:5">
+      <c r="E76" s="16"/>
     </row>
     <row r="77" customFormat="1" spans="1:6">
       <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" t="s">
+        <v>92</v>
+      </c>
+      <c r="E77" s="16">
+        <v>45747</v>
+      </c>
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" customFormat="1" spans="1:6">
+      <c r="A78">
         <v>141</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B78" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" t="s">
         <v>8</v>
       </c>
-      <c r="D77" t="s">
-        <v>94</v>
-      </c>
-      <c r="E77" s="14">
+      <c r="D78" t="s">
+        <v>96</v>
+      </c>
+      <c r="E78" s="16">
         <v>45748</v>
       </c>
-      <c r="F77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" ht="35" customHeight="1" spans="2:2">
-      <c r="B79" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81">
-        <v>226</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C81" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" ht="35" customHeight="1" spans="2:2">
+      <c r="B80" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="E81" s="14">
-        <v>45733</v>
-      </c>
-      <c r="F81" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>101</v>
+        <v>226</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>98</v>
@@ -2787,114 +2805,114 @@
       <c r="D82" t="s">
         <v>99</v>
       </c>
-      <c r="E82" s="14">
+      <c r="E82" s="16">
+        <v>45733</v>
+      </c>
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>101</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>101</v>
+      </c>
+      <c r="E83" s="16">
         <v>45839</v>
       </c>
-      <c r="F82" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" ht="39" customHeight="1" spans="2:2">
-      <c r="B84" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86">
-        <v>704</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C86" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="F83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" ht="39" customHeight="1" spans="2:2">
+      <c r="B85" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="E86" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F86" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D87" t="s">
         <v>104</v>
       </c>
-      <c r="E87" s="14">
+      <c r="E87" s="16">
+        <v>45757</v>
+      </c>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <v>33</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C88" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" t="s">
+        <v>106</v>
+      </c>
+      <c r="E88" s="16">
         <v>45759</v>
       </c>
-      <c r="F87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" ht="32" customHeight="1" spans="2:2">
-      <c r="B89" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" ht="30" customHeight="1" spans="1:6">
-      <c r="A91">
+      <c r="F88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" ht="32" customHeight="1" spans="2:2">
+      <c r="B90" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" ht="30" customHeight="1" spans="1:6">
+      <c r="A92">
         <v>34</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C91" t="s">
-        <v>24</v>
-      </c>
-      <c r="D91" t="s">
-        <v>107</v>
-      </c>
-      <c r="E91" s="14">
+      <c r="B92" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" t="s">
+        <v>109</v>
+      </c>
+      <c r="E92" s="16">
         <v>45773</v>
       </c>
-      <c r="F91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" ht="29" customHeight="1" spans="2:2">
-      <c r="B93" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95">
-        <v>226</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" t="s">
-        <v>109</v>
-      </c>
-      <c r="E95" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F95" t="s">
-        <v>10</v>
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" ht="29" customHeight="1" spans="2:2">
+      <c r="B94" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -2902,8 +2920,8 @@
       <c r="D96" t="s">
         <v>111</v>
       </c>
-      <c r="E96" s="14">
-        <v>45782</v>
+      <c r="E96" s="16">
+        <v>45774</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
@@ -2911,7 +2929,7 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>112</v>
@@ -2922,53 +2940,53 @@
       <c r="D97" t="s">
         <v>113</v>
       </c>
-      <c r="E97" s="14">
+      <c r="E97" s="16">
+        <v>45782</v>
+      </c>
+      <c r="F97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>112</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" t="s">
+        <v>115</v>
+      </c>
+      <c r="E98" s="16">
         <v>45842</v>
       </c>
-      <c r="F97" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2">
-      <c r="B99" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C101" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="F98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="13" t="s">
         <v>116</v>
-      </c>
-      <c r="E101" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F101" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C102" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D102" t="s">
         <v>118</v>
       </c>
-      <c r="E102" s="14">
-        <v>45785</v>
+      <c r="E102" s="16">
+        <v>45784</v>
       </c>
       <c r="F102" t="s">
         <v>10</v>
@@ -2976,7 +2994,7 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>119</v>
@@ -2987,66 +3005,66 @@
       <c r="D103" t="s">
         <v>120</v>
       </c>
-      <c r="E103" s="14">
+      <c r="E103" s="16">
+        <v>45785</v>
+      </c>
+      <c r="F103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>107</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C104" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" t="s">
+        <v>122</v>
+      </c>
+      <c r="E104" s="16">
         <v>45850</v>
       </c>
-      <c r="F103" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="105" ht="27" customHeight="1" spans="2:2">
-      <c r="B105" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107">
+      <c r="F104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" ht="27" customHeight="1" spans="2:2">
+      <c r="B106" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
         <v>235</v>
       </c>
-      <c r="B107" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C107" t="s">
-        <v>24</v>
-      </c>
-      <c r="D107" t="s">
-        <v>123</v>
-      </c>
-      <c r="E107" s="14">
+      <c r="B108" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C108" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" t="s">
+        <v>125</v>
+      </c>
+      <c r="E108" s="16">
         <v>45786</v>
       </c>
-      <c r="F107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" ht="24" customHeight="1" spans="2:2">
-      <c r="B109" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111">
-        <v>133</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C111" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="F108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" ht="24" customHeight="1" spans="2:2">
+      <c r="B110" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="E111" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F111" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>127</v>
@@ -3057,8 +3075,8 @@
       <c r="D112" t="s">
         <v>128</v>
       </c>
-      <c r="E112" s="14">
-        <v>45806</v>
+      <c r="E112" s="16">
+        <v>45791</v>
       </c>
       <c r="F112" t="s">
         <v>10</v>
@@ -3066,7 +3084,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>129</v>
@@ -3077,8 +3095,8 @@
       <c r="D113" t="s">
         <v>130</v>
       </c>
-      <c r="E113" s="14">
-        <v>45807</v>
+      <c r="E113" s="16">
+        <v>45806</v>
       </c>
       <c r="F113" t="s">
         <v>10</v>
@@ -3086,19 +3104,19 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>131</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D114" t="s">
         <v>132</v>
       </c>
-      <c r="E114" s="14">
-        <v>45833</v>
+      <c r="E114" s="16">
+        <v>45807</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
@@ -3106,52 +3124,52 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C115" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D115" t="s">
         <v>134</v>
       </c>
-      <c r="E115" s="14">
+      <c r="E115" s="16">
+        <v>45833</v>
+      </c>
+      <c r="F115" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
+        <v>994</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C116" t="s">
+        <v>24</v>
+      </c>
+      <c r="D116" t="s">
+        <v>136</v>
+      </c>
+      <c r="E116" s="16">
         <v>45834</v>
       </c>
-      <c r="F115" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117" ht="29" customHeight="1" spans="2:2">
-      <c r="B117" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119">
-        <v>106</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C119" t="s">
-        <v>24</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="F116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" ht="29" customHeight="1" spans="2:2">
+      <c r="B118" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="E119" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F119" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>138</v>
@@ -3162,77 +3180,97 @@
       <c r="D120" t="s">
         <v>139</v>
       </c>
-      <c r="E120" s="14">
+      <c r="E120" s="16">
+        <v>45782</v>
+      </c>
+      <c r="F120" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
+        <v>207</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C121" t="s">
+        <v>24</v>
+      </c>
+      <c r="D121" t="s">
+        <v>141</v>
+      </c>
+      <c r="E121" s="16">
         <v>45817</v>
       </c>
-      <c r="F120" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" ht="35" customHeight="1" spans="2:2">
-      <c r="B122" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124">
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" ht="35" customHeight="1" spans="2:2">
+      <c r="B123" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
         <v>127</v>
       </c>
-      <c r="B124" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C124" t="s">
-        <v>142</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="B125" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="E124" s="14">
+      <c r="C125" t="s">
+        <v>144</v>
+      </c>
+      <c r="D125" t="s">
+        <v>145</v>
+      </c>
+      <c r="E125" s="16">
         <v>45831</v>
       </c>
-      <c r="F124" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" ht="41" customHeight="1" spans="1:2">
-      <c r="A130" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B130" s="18">
+      <c r="F125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" ht="41" customHeight="1" spans="1:2">
+      <c r="A131" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131" s="20">
         <f>COUNT(A:A)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="132" ht="30" customHeight="1" spans="1:2">
-      <c r="A132" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B132" s="20">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" ht="30" customHeight="1" spans="1:2">
+      <c r="A133" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B133" s="22">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>25</v>
       </c>
     </row>
-    <row r="133" ht="40" customHeight="1" spans="1:2">
-      <c r="A133" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B133" s="22">
+    <row r="134" ht="40" customHeight="1" spans="1:2">
+      <c r="A134" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B134" s="24">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="134" ht="36" customHeight="1" spans="1:2">
-      <c r="A134" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B134" s="24">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="135" ht="36" customHeight="1" spans="1:2">
+      <c r="A135" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B135" s="26">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B124" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B125" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
docs : updated the tracker sheet
</commit_message>
<xml_diff>
--- a/50  days challenge/DSA_trackerSheet.xlsx
+++ b/50  days challenge/DSA_trackerSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="152">
   <si>
     <t>Q No.</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>DFS ,recursion</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>DFS , height-balanced ,recursion ,flag</t>
   </si>
   <si>
     <t>Binary Search (basic)</t>
@@ -1230,7 +1236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1266,9 +1272,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1852,10 +1855,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1896,7 +1899,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="15"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -1911,7 +1914,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>45688</v>
       </c>
       <c r="F5" t="s">
@@ -1931,7 +1934,7 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>45688</v>
       </c>
       <c r="F6" t="s">
@@ -1951,7 +1954,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>45689</v>
       </c>
       <c r="F7" t="s">
@@ -1971,7 +1974,7 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="15">
         <v>45689</v>
       </c>
       <c r="F8" t="s">
@@ -1991,7 +1994,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>45690</v>
       </c>
       <c r="F9" t="s">
@@ -2011,7 +2014,7 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>45691</v>
       </c>
       <c r="F10" t="s">
@@ -2031,7 +2034,7 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>45692</v>
       </c>
       <c r="F11" t="s">
@@ -2051,7 +2054,7 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>45693</v>
       </c>
       <c r="F12" t="s">
@@ -2076,7 +2079,7 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="15">
         <v>45691</v>
       </c>
       <c r="F16" t="s">
@@ -2096,7 +2099,7 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="15">
         <v>45692</v>
       </c>
       <c r="F17" t="s">
@@ -2116,7 +2119,7 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="15">
         <v>45694</v>
       </c>
       <c r="F18" t="s">
@@ -2136,7 +2139,7 @@
       <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="15">
         <v>45697</v>
       </c>
       <c r="F19" t="s">
@@ -2156,7 +2159,7 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <v>45700</v>
       </c>
       <c r="F20" t="s">
@@ -2176,7 +2179,7 @@
       <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <v>45808</v>
       </c>
       <c r="F21" t="s">
@@ -2201,7 +2204,7 @@
       <c r="D25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="15">
         <v>45693</v>
       </c>
       <c r="F25" t="s">
@@ -2221,7 +2224,7 @@
       <c r="D26" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="15">
         <v>45694</v>
       </c>
       <c r="F26" t="s">
@@ -2241,7 +2244,7 @@
       <c r="D27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="15">
         <v>45826</v>
       </c>
       <c r="F27" t="s">
@@ -2261,7 +2264,7 @@
       <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="15">
         <v>45827</v>
       </c>
       <c r="F28" t="s">
@@ -2286,7 +2289,7 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="15">
         <v>45695</v>
       </c>
       <c r="F32" t="s">
@@ -2306,7 +2309,7 @@
       <c r="D33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="15">
         <v>45699</v>
       </c>
       <c r="F33" t="s">
@@ -2326,7 +2329,7 @@
       <c r="D34" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="15">
         <v>45746</v>
       </c>
       <c r="F34" t="s">
@@ -2346,7 +2349,7 @@
       <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="15">
         <v>45851</v>
       </c>
       <c r="F35" t="s">
@@ -2374,7 +2377,7 @@
       <c r="D39" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="15">
         <v>45700</v>
       </c>
       <c r="F39" t="s">
@@ -2394,7 +2397,7 @@
       <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="15">
         <v>45701</v>
       </c>
       <c r="F40" t="s">
@@ -2414,7 +2417,7 @@
       <c r="D41" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="16">
+      <c r="E41" s="15">
         <v>45826</v>
       </c>
       <c r="F41" t="s">
@@ -2434,7 +2437,7 @@
       <c r="D42" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="16">
+      <c r="E42" s="15">
         <v>45838</v>
       </c>
       <c r="F42" t="s">
@@ -2443,7 +2446,7 @@
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="11"/>
-      <c r="E43" s="16"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" ht="39" customHeight="1" spans="2:2">
       <c r="B44" s="4" t="s">
@@ -2454,7 +2457,7 @@
       <c r="A46">
         <v>424</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C46" t="s">
@@ -2463,7 +2466,7 @@
       <c r="D46" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E46" s="15">
         <v>45716</v>
       </c>
       <c r="F46" t="s">
@@ -2483,7 +2486,7 @@
       <c r="D47" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="16">
+      <c r="E47" s="15">
         <v>45771</v>
       </c>
       <c r="F47" t="s">
@@ -2503,7 +2506,7 @@
       <c r="D48" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="15">
         <v>45776</v>
       </c>
       <c r="F48" t="s">
@@ -2523,7 +2526,7 @@
       <c r="D49" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="16">
+      <c r="E49" s="15">
         <v>45847</v>
       </c>
       <c r="F49" t="s">
@@ -2531,7 +2534,7 @@
       </c>
     </row>
     <row r="51" ht="31" customHeight="1" spans="2:2">
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2548,7 +2551,7 @@
       <c r="D53" t="s">
         <v>72</v>
       </c>
-      <c r="E53" s="16">
+      <c r="E53" s="15">
         <v>45701</v>
       </c>
       <c r="F53" t="s">
@@ -2568,7 +2571,7 @@
       <c r="D54" t="s">
         <v>74</v>
       </c>
-      <c r="E54" s="16">
+      <c r="E54" s="15">
         <v>45836</v>
       </c>
       <c r="F54" t="s">
@@ -2576,7 +2579,7 @@
       </c>
     </row>
     <row r="56" ht="38" customHeight="1" spans="2:2">
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="12" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2593,7 +2596,7 @@
       <c r="D58" t="s">
         <v>77</v>
       </c>
-      <c r="E58" s="16">
+      <c r="E58" s="15">
         <v>45719</v>
       </c>
       <c r="F58" t="s">
@@ -2613,7 +2616,7 @@
       <c r="D59" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="16">
+      <c r="E59" s="15">
         <v>45731</v>
       </c>
       <c r="F59" t="s">
@@ -2621,7 +2624,7 @@
       </c>
     </row>
     <row r="61" ht="40" customHeight="1" spans="2:2">
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="12" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2638,7 +2641,7 @@
       <c r="D63" t="s">
         <v>82</v>
       </c>
-      <c r="E63" s="16">
+      <c r="E63" s="15">
         <v>45732</v>
       </c>
       <c r="F63" t="s">
@@ -2646,19 +2649,19 @@
       </c>
     </row>
     <row r="64" s="1" customFormat="1" spans="1:6">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>84</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="16">
         <v>45745</v>
       </c>
       <c r="F64" t="s">
@@ -2666,7 +2669,7 @@
       </c>
     </row>
     <row r="66" ht="34" customHeight="1" spans="2:2">
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="12" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2683,7 +2686,7 @@
       <c r="D68" t="s">
         <v>87</v>
       </c>
-      <c r="E68" s="16">
+      <c r="E68" s="15">
         <v>45841</v>
       </c>
       <c r="F68" t="s">
@@ -2708,7 +2711,7 @@
       <c r="D72" t="s">
         <v>90</v>
       </c>
-      <c r="E72" s="16">
+      <c r="E72" s="15">
         <v>45746</v>
       </c>
       <c r="F72" t="s">
@@ -2728,7 +2731,7 @@
       <c r="D73" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="16">
+      <c r="E73" s="15">
         <v>45747</v>
       </c>
       <c r="F73" t="s">
@@ -2736,16 +2739,16 @@
       </c>
     </row>
     <row r="74" customFormat="1" spans="5:5">
-      <c r="E74" s="16"/>
+      <c r="E74" s="15"/>
     </row>
     <row r="75" customFormat="1" ht="26" customHeight="1" spans="2:5">
       <c r="B75" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E75" s="16"/>
+      <c r="E75" s="15"/>
     </row>
     <row r="76" customFormat="1" spans="5:5">
-      <c r="E76" s="16"/>
+      <c r="E76" s="15"/>
     </row>
     <row r="77" customFormat="1" spans="1:6">
       <c r="A77">
@@ -2760,7 +2763,7 @@
       <c r="D77" t="s">
         <v>92</v>
       </c>
-      <c r="E77" s="16">
+      <c r="E77" s="15">
         <v>45747</v>
       </c>
       <c r="F77" t="s">
@@ -2780,7 +2783,7 @@
       <c r="D78" t="s">
         <v>96</v>
       </c>
-      <c r="E78" s="16">
+      <c r="E78" s="15">
         <v>45748</v>
       </c>
       <c r="F78" t="s">
@@ -2788,7 +2791,7 @@
       </c>
     </row>
     <row r="80" ht="35" customHeight="1" spans="2:2">
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="12" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2805,7 +2808,7 @@
       <c r="D82" t="s">
         <v>99</v>
       </c>
-      <c r="E82" s="16">
+      <c r="E82" s="15">
         <v>45733</v>
       </c>
       <c r="F82" t="s">
@@ -2825,114 +2828,114 @@
       <c r="D83" t="s">
         <v>101</v>
       </c>
-      <c r="E83" s="16">
+      <c r="E83" s="15">
         <v>45839</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="85" ht="39" customHeight="1" spans="2:2">
-      <c r="B85" s="13" t="s">
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <v>110</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87">
-        <v>704</v>
-      </c>
-      <c r="B87" s="5" t="s">
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
         <v>103</v>
       </c>
-      <c r="C87" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E84" s="15">
+        <v>45856</v>
+      </c>
+      <c r="F84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" ht="39" customHeight="1" spans="2:2">
+      <c r="B86" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="E87" s="16">
-        <v>45757</v>
-      </c>
-      <c r="F87" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C88" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D88" t="s">
         <v>106</v>
       </c>
-      <c r="E88" s="16">
+      <c r="E88" s="15">
+        <v>45757</v>
+      </c>
+      <c r="F88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89">
+        <v>33</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" t="s">
+        <v>108</v>
+      </c>
+      <c r="E89" s="15">
         <v>45759</v>
       </c>
-      <c r="F88" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" ht="32" customHeight="1" spans="2:2">
-      <c r="B90" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="92" ht="30" customHeight="1" spans="1:6">
-      <c r="A92">
+      <c r="F89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" ht="32" customHeight="1" spans="2:2">
+      <c r="B91" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" ht="30" customHeight="1" spans="1:6">
+      <c r="A93">
         <v>34</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B93" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C93" t="s">
         <v>24</v>
       </c>
-      <c r="D92" t="s">
-        <v>109</v>
-      </c>
-      <c r="E92" s="16">
+      <c r="D93" t="s">
+        <v>111</v>
+      </c>
+      <c r="E93" s="15">
         <v>45773</v>
       </c>
-      <c r="F92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" ht="29" customHeight="1" spans="2:2">
-      <c r="B94" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96">
-        <v>226</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" t="s">
-        <v>111</v>
-      </c>
-      <c r="E96" s="16">
-        <v>45774</v>
-      </c>
-      <c r="F96" t="s">
-        <v>10</v>
+      <c r="F93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" ht="29" customHeight="1" spans="2:2">
+      <c r="B95" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -2940,8 +2943,8 @@
       <c r="D97" t="s">
         <v>113</v>
       </c>
-      <c r="E97" s="16">
-        <v>45782</v>
+      <c r="E97" s="15">
+        <v>45774</v>
       </c>
       <c r="F97" t="s">
         <v>10</v>
@@ -2949,7 +2952,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>114</v>
@@ -2960,53 +2963,53 @@
       <c r="D98" t="s">
         <v>115</v>
       </c>
-      <c r="E98" s="16">
+      <c r="E98" s="15">
+        <v>45782</v>
+      </c>
+      <c r="F98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>112</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" t="s">
+        <v>117</v>
+      </c>
+      <c r="E99" s="15">
         <v>45842</v>
       </c>
-      <c r="F98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2">
-      <c r="B100" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102">
-        <v>100</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C102" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="F99" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="E102" s="16">
-        <v>45784</v>
-      </c>
-      <c r="F102" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C103" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D103" t="s">
         <v>120</v>
       </c>
-      <c r="E103" s="16">
-        <v>45785</v>
+      <c r="E103" s="15">
+        <v>45784</v>
       </c>
       <c r="F103" t="s">
         <v>10</v>
@@ -3014,7 +3017,7 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>121</v>
@@ -3025,66 +3028,66 @@
       <c r="D104" t="s">
         <v>122</v>
       </c>
-      <c r="E104" s="16">
+      <c r="E104" s="15">
+        <v>45785</v>
+      </c>
+      <c r="F104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105">
+        <v>107</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C105" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" t="s">
+        <v>124</v>
+      </c>
+      <c r="E105" s="15">
         <v>45850</v>
       </c>
-      <c r="F104" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" ht="27" customHeight="1" spans="2:2">
-      <c r="B106" s="13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108">
+      <c r="F105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" ht="27" customHeight="1" spans="2:2">
+      <c r="B107" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
         <v>235</v>
       </c>
-      <c r="B108" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C108" t="s">
+      <c r="B109" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C109" t="s">
         <v>24</v>
       </c>
-      <c r="D108" t="s">
-        <v>125</v>
-      </c>
-      <c r="E108" s="16">
+      <c r="D109" t="s">
+        <v>127</v>
+      </c>
+      <c r="E109" s="15">
         <v>45786</v>
       </c>
-      <c r="F108" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" ht="24" customHeight="1" spans="2:2">
-      <c r="B110" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112">
-        <v>133</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C112" t="s">
-        <v>24</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" ht="24" customHeight="1" spans="2:2">
+      <c r="B111" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="E112" s="16">
-        <v>45791</v>
-      </c>
-      <c r="F112" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>129</v>
@@ -3095,8 +3098,8 @@
       <c r="D113" t="s">
         <v>130</v>
       </c>
-      <c r="E113" s="16">
-        <v>45806</v>
+      <c r="E113" s="15">
+        <v>45791</v>
       </c>
       <c r="F113" t="s">
         <v>10</v>
@@ -3104,7 +3107,7 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>131</v>
@@ -3115,8 +3118,8 @@
       <c r="D114" t="s">
         <v>132</v>
       </c>
-      <c r="E114" s="16">
-        <v>45807</v>
+      <c r="E114" s="15">
+        <v>45806</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
@@ -3124,19 +3127,19 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C115" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D115" t="s">
         <v>134</v>
       </c>
-      <c r="E115" s="16">
-        <v>45833</v>
+      <c r="E115" s="15">
+        <v>45807</v>
       </c>
       <c r="F115" t="s">
         <v>10</v>
@@ -3144,52 +3147,52 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>135</v>
       </c>
       <c r="C116" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D116" t="s">
         <v>136</v>
       </c>
-      <c r="E116" s="16">
+      <c r="E116" s="15">
+        <v>45833</v>
+      </c>
+      <c r="F116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117">
+        <v>994</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C117" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" t="s">
+        <v>138</v>
+      </c>
+      <c r="E117" s="15">
         <v>45834</v>
       </c>
-      <c r="F116" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="118" ht="29" customHeight="1" spans="2:2">
-      <c r="B118" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120">
-        <v>106</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C120" t="s">
-        <v>24</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="F117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" ht="29" customHeight="1" spans="2:2">
+      <c r="B119" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E120" s="16">
-        <v>45782</v>
-      </c>
-      <c r="F120" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>140</v>
@@ -3200,77 +3203,97 @@
       <c r="D121" t="s">
         <v>141</v>
       </c>
-      <c r="E121" s="16">
+      <c r="E121" s="15">
+        <v>45782</v>
+      </c>
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122">
+        <v>207</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C122" t="s">
+        <v>24</v>
+      </c>
+      <c r="D122" t="s">
+        <v>143</v>
+      </c>
+      <c r="E122" s="15">
         <v>45817</v>
       </c>
-      <c r="F121" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="123" ht="35" customHeight="1" spans="2:2">
-      <c r="B123" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125">
+      <c r="F122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" ht="35" customHeight="1" spans="2:2">
+      <c r="B124" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
         <v>127</v>
       </c>
-      <c r="B125" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C125" t="s">
-        <v>144</v>
-      </c>
-      <c r="D125" t="s">
+      <c r="B126" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E125" s="16">
+      <c r="C126" t="s">
+        <v>146</v>
+      </c>
+      <c r="D126" t="s">
+        <v>147</v>
+      </c>
+      <c r="E126" s="15">
         <v>45831</v>
       </c>
-      <c r="F125" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="131" ht="41" customHeight="1" spans="1:2">
-      <c r="A131" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B131" s="20">
+      <c r="F126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" ht="41" customHeight="1" spans="1:2">
+      <c r="A132" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B132" s="19">
         <f>COUNT(A:A)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="133" ht="30" customHeight="1" spans="1:2">
-      <c r="A133" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B133" s="22">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="134" ht="30" customHeight="1" spans="1:2">
+      <c r="A134" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B134" s="21">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="134" ht="40" customHeight="1" spans="1:2">
-      <c r="A134" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B134" s="24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" ht="40" customHeight="1" spans="1:2">
+      <c r="A135" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" s="23">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>34</v>
       </c>
     </row>
-    <row r="135" ht="36" customHeight="1" spans="1:2">
-      <c r="A135" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B135" s="26">
+    <row r="136" ht="36" customHeight="1" spans="1:2">
+      <c r="A136" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B136" s="25">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B125" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B126" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
111. Minimum Depth of Binary Tree
</commit_message>
<xml_diff>
--- a/50  days challenge/DSA_trackerSheet.xlsx
+++ b/50  days challenge/DSA_trackerSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="154">
   <si>
     <t>Q No.</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>DFS , height-balanced ,recursion ,flag</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>DFS .recursion</t>
   </si>
   <si>
     <t>Binary Search (basic)</t>
@@ -1855,10 +1861,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2855,107 +2861,107 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" ht="39" customHeight="1" spans="2:2">
-      <c r="B86" s="12" t="s">
+    <row r="85" spans="1:6">
+      <c r="A85">
+        <v>111</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88">
-        <v>704</v>
-      </c>
-      <c r="B88" s="5" t="s">
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
         <v>105</v>
       </c>
-      <c r="C88" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E85" s="15">
+        <v>45858</v>
+      </c>
+      <c r="F85" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" ht="39" customHeight="1" spans="2:2">
+      <c r="B87" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="E88" s="15">
-        <v>45757</v>
-      </c>
-      <c r="F88" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C89" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D89" t="s">
         <v>108</v>
       </c>
       <c r="E89" s="15">
+        <v>45757</v>
+      </c>
+      <c r="F89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90">
+        <v>33</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" t="s">
+        <v>110</v>
+      </c>
+      <c r="E90" s="15">
         <v>45759</v>
       </c>
-      <c r="F89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" ht="32" customHeight="1" spans="2:2">
-      <c r="B91" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="93" ht="30" customHeight="1" spans="1:6">
-      <c r="A93">
+      <c r="F90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" ht="32" customHeight="1" spans="2:2">
+      <c r="B92" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="94" ht="30" customHeight="1" spans="1:6">
+      <c r="A94">
         <v>34</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="B94" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C94" t="s">
         <v>24</v>
       </c>
-      <c r="D93" t="s">
-        <v>111</v>
-      </c>
-      <c r="E93" s="15">
+      <c r="D94" t="s">
+        <v>113</v>
+      </c>
+      <c r="E94" s="15">
         <v>45773</v>
       </c>
-      <c r="F93" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" ht="29" customHeight="1" spans="2:2">
-      <c r="B95" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97">
-        <v>226</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C97" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" t="s">
-        <v>113</v>
-      </c>
-      <c r="E97" s="15">
-        <v>45774</v>
-      </c>
-      <c r="F97" t="s">
-        <v>10</v>
+      <c r="F94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" ht="29" customHeight="1" spans="2:2">
+      <c r="B96" s="12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -2964,7 +2970,7 @@
         <v>115</v>
       </c>
       <c r="E98" s="15">
-        <v>45782</v>
+        <v>45774</v>
       </c>
       <c r="F98" t="s">
         <v>10</v>
@@ -2972,7 +2978,7 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>116</v>
@@ -2984,52 +2990,52 @@
         <v>117</v>
       </c>
       <c r="E99" s="15">
+        <v>45782</v>
+      </c>
+      <c r="F99" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>112</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" t="s">
+        <v>119</v>
+      </c>
+      <c r="E100" s="15">
         <v>45842</v>
       </c>
-      <c r="F99" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2">
-      <c r="B101" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103">
-        <v>100</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C103" t="s">
-        <v>8</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="12" t="s">
         <v>120</v>
-      </c>
-      <c r="E103" s="15">
-        <v>45784</v>
-      </c>
-      <c r="F103" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C104" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D104" t="s">
         <v>122</v>
       </c>
       <c r="E104" s="15">
-        <v>45785</v>
+        <v>45784</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -3037,7 +3043,7 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>123</v>
@@ -3049,65 +3055,65 @@
         <v>124</v>
       </c>
       <c r="E105" s="15">
+        <v>45785</v>
+      </c>
+      <c r="F105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106">
+        <v>107</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C106" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" t="s">
+        <v>126</v>
+      </c>
+      <c r="E106" s="15">
         <v>45850</v>
       </c>
-      <c r="F105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" ht="27" customHeight="1" spans="2:2">
-      <c r="B107" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109">
+      <c r="F106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" ht="27" customHeight="1" spans="2:2">
+      <c r="B108" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110">
         <v>235</v>
       </c>
-      <c r="B109" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="B110" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C110" t="s">
         <v>24</v>
       </c>
-      <c r="D109" t="s">
-        <v>127</v>
-      </c>
-      <c r="E109" s="15">
+      <c r="D110" t="s">
+        <v>129</v>
+      </c>
+      <c r="E110" s="15">
         <v>45786</v>
       </c>
-      <c r="F109" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="111" ht="24" customHeight="1" spans="2:2">
-      <c r="B111" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113">
-        <v>133</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C113" t="s">
-        <v>24</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="F110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" ht="24" customHeight="1" spans="2:2">
+      <c r="B112" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="E113" s="15">
-        <v>45791</v>
-      </c>
-      <c r="F113" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>131</v>
@@ -3119,7 +3125,7 @@
         <v>132</v>
       </c>
       <c r="E114" s="15">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
@@ -3127,7 +3133,7 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>133</v>
@@ -3139,7 +3145,7 @@
         <v>134</v>
       </c>
       <c r="E115" s="15">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F115" t="s">
         <v>10</v>
@@ -3147,19 +3153,19 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>135</v>
       </c>
       <c r="C116" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D116" t="s">
         <v>136</v>
       </c>
       <c r="E116" s="15">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F116" t="s">
         <v>10</v>
@@ -3167,52 +3173,52 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C117" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D117" t="s">
         <v>138</v>
       </c>
       <c r="E117" s="15">
+        <v>45833</v>
+      </c>
+      <c r="F117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118">
+        <v>994</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118" t="s">
+        <v>24</v>
+      </c>
+      <c r="D118" t="s">
+        <v>140</v>
+      </c>
+      <c r="E118" s="15">
         <v>45834</v>
       </c>
-      <c r="F117" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" ht="29" customHeight="1" spans="2:2">
-      <c r="B119" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121">
-        <v>106</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C121" t="s">
-        <v>24</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" ht="29" customHeight="1" spans="2:2">
+      <c r="B120" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="E121" s="15">
-        <v>45782</v>
-      </c>
-      <c r="F121" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>142</v>
@@ -3224,76 +3230,96 @@
         <v>143</v>
       </c>
       <c r="E122" s="15">
+        <v>45782</v>
+      </c>
+      <c r="F122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
+        <v>207</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C123" t="s">
+        <v>24</v>
+      </c>
+      <c r="D123" t="s">
+        <v>145</v>
+      </c>
+      <c r="E123" s="15">
         <v>45817</v>
       </c>
-      <c r="F122" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="124" ht="35" customHeight="1" spans="2:2">
-      <c r="B124" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126">
+      <c r="F123" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" ht="35" customHeight="1" spans="2:2">
+      <c r="B125" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127">
         <v>127</v>
       </c>
-      <c r="B126" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C126" t="s">
-        <v>146</v>
-      </c>
-      <c r="D126" t="s">
+      <c r="B127" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="E126" s="15">
+      <c r="C127" t="s">
+        <v>148</v>
+      </c>
+      <c r="D127" t="s">
+        <v>149</v>
+      </c>
+      <c r="E127" s="15">
         <v>45831</v>
       </c>
-      <c r="F126" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="132" ht="41" customHeight="1" spans="1:2">
-      <c r="A132" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B132" s="19">
+      <c r="F127" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" ht="41" customHeight="1" spans="1:2">
+      <c r="A133" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B133" s="19">
         <f>COUNT(A:A)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="134" ht="30" customHeight="1" spans="1:2">
-      <c r="A134" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B134" s="21">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="135" ht="30" customHeight="1" spans="1:2">
+      <c r="A135" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B135" s="21">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="135" ht="40" customHeight="1" spans="1:2">
-      <c r="A135" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="B135" s="23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="136" ht="40" customHeight="1" spans="1:2">
+      <c r="A136" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B136" s="23">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>34</v>
       </c>
     </row>
-    <row r="136" ht="36" customHeight="1" spans="1:2">
-      <c r="A136" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="B136" s="25">
+    <row r="137" ht="36" customHeight="1" spans="1:2">
+      <c r="A137" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B137" s="25">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B127" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Docs: updated the tracker sheet
</commit_message>
<xml_diff>
--- a/50  days challenge/DSA_trackerSheet.xlsx
+++ b/50  days challenge/DSA_trackerSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="156">
   <si>
     <t>Q No.</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>DFS .recursion</t>
+  </si>
+  <si>
+    <t>Binary Tree Preorder Traversal</t>
+  </si>
+  <si>
+    <t>DFS</t>
   </si>
   <si>
     <t>Binary Search (basic)</t>
@@ -1861,10 +1867,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2881,107 +2887,107 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" ht="39" customHeight="1" spans="2:2">
-      <c r="B87" s="12" t="s">
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <v>144</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89">
-        <v>704</v>
-      </c>
-      <c r="B89" s="5" t="s">
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
         <v>107</v>
       </c>
-      <c r="C89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E86" s="15">
+        <v>45871</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" ht="39" customHeight="1" spans="2:2">
+      <c r="B88" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="E89" s="15">
-        <v>45757</v>
-      </c>
-      <c r="F89" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C90" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D90" t="s">
         <v>110</v>
       </c>
       <c r="E90" s="15">
+        <v>45757</v>
+      </c>
+      <c r="F90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>33</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C91" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" t="s">
+        <v>112</v>
+      </c>
+      <c r="E91" s="15">
         <v>45759</v>
       </c>
-      <c r="F90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" ht="32" customHeight="1" spans="2:2">
-      <c r="B92" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="94" ht="30" customHeight="1" spans="1:6">
-      <c r="A94">
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" ht="32" customHeight="1" spans="2:2">
+      <c r="B93" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="95" ht="30" customHeight="1" spans="1:6">
+      <c r="A95">
         <v>34</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="B95" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C95" t="s">
         <v>24</v>
       </c>
-      <c r="D94" t="s">
-        <v>113</v>
-      </c>
-      <c r="E94" s="15">
+      <c r="D95" t="s">
+        <v>115</v>
+      </c>
+      <c r="E95" s="15">
         <v>45773</v>
       </c>
-      <c r="F94" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" ht="29" customHeight="1" spans="2:2">
-      <c r="B96" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98">
-        <v>226</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C98" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98" t="s">
-        <v>115</v>
-      </c>
-      <c r="E98" s="15">
-        <v>45774</v>
-      </c>
-      <c r="F98" t="s">
-        <v>10</v>
+      <c r="F95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" ht="29" customHeight="1" spans="2:2">
+      <c r="B97" s="12" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -2990,7 +2996,7 @@
         <v>117</v>
       </c>
       <c r="E99" s="15">
-        <v>45782</v>
+        <v>45774</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -2998,7 +3004,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>118</v>
@@ -3010,52 +3016,52 @@
         <v>119</v>
       </c>
       <c r="E100" s="15">
+        <v>45782</v>
+      </c>
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>112</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>121</v>
+      </c>
+      <c r="E101" s="15">
         <v>45842</v>
       </c>
-      <c r="F100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2">
-      <c r="B102" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104">
-        <v>100</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C104" t="s">
-        <v>8</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="F101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="E104" s="15">
-        <v>45784</v>
-      </c>
-      <c r="F104" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D105" t="s">
         <v>124</v>
       </c>
       <c r="E105" s="15">
-        <v>45785</v>
+        <v>45784</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -3063,7 +3069,7 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>125</v>
@@ -3075,65 +3081,65 @@
         <v>126</v>
       </c>
       <c r="E106" s="15">
+        <v>45785</v>
+      </c>
+      <c r="F106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C107" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" t="s">
+        <v>128</v>
+      </c>
+      <c r="E107" s="15">
         <v>45850</v>
       </c>
-      <c r="F106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" ht="27" customHeight="1" spans="2:2">
-      <c r="B108" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110">
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" ht="27" customHeight="1" spans="2:2">
+      <c r="B109" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111">
         <v>235</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="B111" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C111" t="s">
         <v>24</v>
       </c>
-      <c r="D110" t="s">
-        <v>129</v>
-      </c>
-      <c r="E110" s="15">
+      <c r="D111" t="s">
+        <v>131</v>
+      </c>
+      <c r="E111" s="15">
         <v>45786</v>
       </c>
-      <c r="F110" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" ht="24" customHeight="1" spans="2:2">
-      <c r="B112" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114">
-        <v>133</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C114" t="s">
-        <v>24</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="F111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" ht="24" customHeight="1" spans="2:2">
+      <c r="B113" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="E114" s="15">
-        <v>45791</v>
-      </c>
-      <c r="F114" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>133</v>
@@ -3145,7 +3151,7 @@
         <v>134</v>
       </c>
       <c r="E115" s="15">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F115" t="s">
         <v>10</v>
@@ -3153,7 +3159,7 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>135</v>
@@ -3165,7 +3171,7 @@
         <v>136</v>
       </c>
       <c r="E116" s="15">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F116" t="s">
         <v>10</v>
@@ -3173,19 +3179,19 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C117" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D117" t="s">
         <v>138</v>
       </c>
       <c r="E117" s="15">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
@@ -3193,52 +3199,52 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C118" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D118" t="s">
         <v>140</v>
       </c>
       <c r="E118" s="15">
+        <v>45833</v>
+      </c>
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119">
+        <v>994</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C119" t="s">
+        <v>24</v>
+      </c>
+      <c r="D119" t="s">
+        <v>142</v>
+      </c>
+      <c r="E119" s="15">
         <v>45834</v>
       </c>
-      <c r="F118" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" ht="29" customHeight="1" spans="2:2">
-      <c r="B120" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122">
-        <v>106</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C122" t="s">
-        <v>24</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="F119" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" ht="29" customHeight="1" spans="2:2">
+      <c r="B121" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="E122" s="15">
-        <v>45782</v>
-      </c>
-      <c r="F122" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>144</v>
@@ -3250,76 +3256,96 @@
         <v>145</v>
       </c>
       <c r="E123" s="15">
+        <v>45782</v>
+      </c>
+      <c r="F123" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124">
+        <v>207</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C124" t="s">
+        <v>24</v>
+      </c>
+      <c r="D124" t="s">
+        <v>147</v>
+      </c>
+      <c r="E124" s="15">
         <v>45817</v>
       </c>
-      <c r="F123" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="125" ht="35" customHeight="1" spans="2:2">
-      <c r="B125" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127">
+      <c r="F124" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" ht="35" customHeight="1" spans="2:2">
+      <c r="B126" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128">
         <v>127</v>
       </c>
-      <c r="B127" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C127" t="s">
-        <v>148</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="B128" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E127" s="15">
+      <c r="C128" t="s">
+        <v>150</v>
+      </c>
+      <c r="D128" t="s">
+        <v>151</v>
+      </c>
+      <c r="E128" s="15">
         <v>45831</v>
       </c>
-      <c r="F127" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" ht="41" customHeight="1" spans="1:2">
-      <c r="A133" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="B133" s="19">
+      <c r="F128" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" ht="41" customHeight="1" spans="1:2">
+      <c r="A134" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B134" s="19">
         <f>COUNT(A:A)</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="135" ht="30" customHeight="1" spans="1:2">
-      <c r="A135" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B135" s="21">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="136" ht="30" customHeight="1" spans="1:2">
+      <c r="A136" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B136" s="21">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="136" ht="40" customHeight="1" spans="1:2">
-      <c r="A136" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B136" s="23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="137" ht="40" customHeight="1" spans="1:2">
+      <c r="A137" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B137" s="23">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>34</v>
       </c>
     </row>
-    <row r="137" ht="36" customHeight="1" spans="1:2">
-      <c r="A137" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="B137" s="25">
+    <row r="138" ht="36" customHeight="1" spans="1:2">
+      <c r="A138" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B138" s="25">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B127" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B128" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
219. Contains Duplicate II (Sliding window)
</commit_message>
<xml_diff>
--- a/50  days challenge/DSA_trackerSheet.xlsx
+++ b/50  days challenge/DSA_trackerSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="158">
   <si>
     <t>Q No.</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>Reschedule Meetings for Maximum Free Time I</t>
+  </si>
+  <si>
+    <t>Contains Duplicate II</t>
+  </si>
+  <si>
+    <t>Arrays,sliding window,hashmap</t>
   </si>
   <si>
     <t>Heap (Basics)</t>
@@ -1288,13 +1294,13 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1867,10 +1873,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1911,7 +1917,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="14"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -1926,7 +1932,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>45688</v>
       </c>
       <c r="F5" t="s">
@@ -1946,7 +1952,7 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>45688</v>
       </c>
       <c r="F6" t="s">
@@ -1966,7 +1972,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>45689</v>
       </c>
       <c r="F7" t="s">
@@ -1986,7 +1992,7 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>45689</v>
       </c>
       <c r="F8" t="s">
@@ -2006,7 +2012,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>45690</v>
       </c>
       <c r="F9" t="s">
@@ -2026,7 +2032,7 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>45691</v>
       </c>
       <c r="F10" t="s">
@@ -2046,7 +2052,7 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>45692</v>
       </c>
       <c r="F11" t="s">
@@ -2066,7 +2072,7 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>45693</v>
       </c>
       <c r="F12" t="s">
@@ -2091,7 +2097,7 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>45691</v>
       </c>
       <c r="F16" t="s">
@@ -2111,7 +2117,7 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>45692</v>
       </c>
       <c r="F17" t="s">
@@ -2131,7 +2137,7 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <v>45694</v>
       </c>
       <c r="F18" t="s">
@@ -2151,7 +2157,7 @@
       <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <v>45697</v>
       </c>
       <c r="F19" t="s">
@@ -2171,7 +2177,7 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="14">
         <v>45700</v>
       </c>
       <c r="F20" t="s">
@@ -2191,7 +2197,7 @@
       <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>45808</v>
       </c>
       <c r="F21" t="s">
@@ -2216,7 +2222,7 @@
       <c r="D25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>45693</v>
       </c>
       <c r="F25" t="s">
@@ -2236,7 +2242,7 @@
       <c r="D26" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="14">
         <v>45694</v>
       </c>
       <c r="F26" t="s">
@@ -2256,7 +2262,7 @@
       <c r="D27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="14">
         <v>45826</v>
       </c>
       <c r="F27" t="s">
@@ -2276,7 +2282,7 @@
       <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="14">
         <v>45827</v>
       </c>
       <c r="F28" t="s">
@@ -2301,7 +2307,7 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="14">
         <v>45695</v>
       </c>
       <c r="F32" t="s">
@@ -2321,7 +2327,7 @@
       <c r="D33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="14">
         <v>45699</v>
       </c>
       <c r="F33" t="s">
@@ -2341,7 +2347,7 @@
       <c r="D34" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="14">
         <v>45746</v>
       </c>
       <c r="F34" t="s">
@@ -2361,7 +2367,7 @@
       <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="14">
         <v>45851</v>
       </c>
       <c r="F35" t="s">
@@ -2389,7 +2395,7 @@
       <c r="D39" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="14">
         <v>45700</v>
       </c>
       <c r="F39" t="s">
@@ -2409,7 +2415,7 @@
       <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="14">
         <v>45701</v>
       </c>
       <c r="F40" t="s">
@@ -2429,7 +2435,7 @@
       <c r="D41" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="14">
         <v>45826</v>
       </c>
       <c r="F41" t="s">
@@ -2449,7 +2455,7 @@
       <c r="D42" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="14">
         <v>45838</v>
       </c>
       <c r="F42" t="s">
@@ -2458,7 +2464,7 @@
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="11"/>
-      <c r="E43" s="15"/>
+      <c r="E43" s="14"/>
     </row>
     <row r="44" ht="39" customHeight="1" spans="2:2">
       <c r="B44" s="4" t="s">
@@ -2478,7 +2484,7 @@
       <c r="D46" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="14">
         <v>45716</v>
       </c>
       <c r="F46" t="s">
@@ -2498,7 +2504,7 @@
       <c r="D47" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="14">
         <v>45771</v>
       </c>
       <c r="F47" t="s">
@@ -2518,7 +2524,7 @@
       <c r="D48" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="14">
         <v>45776</v>
       </c>
       <c r="F48" t="s">
@@ -2538,203 +2544,203 @@
       <c r="D49" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="14">
         <v>45847</v>
       </c>
       <c r="F49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" ht="31" customHeight="1" spans="2:2">
-      <c r="B51" s="12" t="s">
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>219</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>3066</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
         <v>71</v>
       </c>
-      <c r="C53" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="E50" s="14">
+        <v>45872</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" ht="31" customHeight="1" spans="2:2">
+      <c r="B52" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E53" s="15">
-        <v>45701</v>
-      </c>
-      <c r="F53" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>2099</v>
+        <v>3066</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
         <v>74</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="14">
+        <v>45701</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>2099</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="14">
         <v>45836</v>
       </c>
-      <c r="F54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" ht="38" customHeight="1" spans="2:2">
-      <c r="B56" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58">
-        <v>20</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" ht="38" customHeight="1" spans="2:2">
+      <c r="B57" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="E58" s="15">
-        <v>45719</v>
-      </c>
-      <c r="F58" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="14">
+        <v>45719</v>
+      </c>
+      <c r="F59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>155</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="14">
         <v>45731</v>
       </c>
-      <c r="F59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" ht="40" customHeight="1" spans="2:2">
-      <c r="B61" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63">
+      <c r="F60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" ht="40" customHeight="1" spans="2:2">
+      <c r="B62" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
         <v>739</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" t="s">
-        <v>82</v>
-      </c>
-      <c r="E63" s="15">
-        <v>45732</v>
-      </c>
-      <c r="F63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" s="1" customFormat="1" spans="1:6">
-      <c r="A64" s="13">
-        <v>84</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E64" s="16">
+      <c r="E64" s="14">
+        <v>45732</v>
+      </c>
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" s="1" customFormat="1" spans="1:6">
+      <c r="A65" s="15">
+        <v>84</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" s="16">
         <v>45745</v>
       </c>
-      <c r="F64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" ht="34" customHeight="1" spans="2:2">
-      <c r="B66" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="68" ht="18" spans="1:6">
-      <c r="A68">
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" ht="34" customHeight="1" spans="2:2">
+      <c r="B67" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" ht="18" spans="1:6">
+      <c r="A69">
         <v>225</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B69" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" t="s">
         <v>8</v>
       </c>
-      <c r="D68" t="s">
-        <v>87</v>
-      </c>
-      <c r="E68" s="15">
+      <c r="D69" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69" s="14">
         <v>45841</v>
       </c>
-      <c r="F68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B70" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="72" customFormat="1" ht="18" spans="1:6">
-      <c r="A72">
+      <c r="F69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B71" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" ht="18" spans="1:6">
+      <c r="A73">
         <v>206</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C72" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" t="s">
-        <v>90</v>
-      </c>
-      <c r="E72" s="15">
-        <v>45746</v>
-      </c>
-      <c r="F72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" customFormat="1" spans="1:6">
-      <c r="A73">
-        <v>21</v>
-      </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="10" t="s">
         <v>91</v>
       </c>
       <c r="C73" t="s">
@@ -2743,93 +2749,93 @@
       <c r="D73" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="15">
+      <c r="E73" s="14">
+        <v>45746</v>
+      </c>
+      <c r="F73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" spans="1:6">
+      <c r="A74">
+        <v>21</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>94</v>
+      </c>
+      <c r="E74" s="14">
         <v>45747</v>
       </c>
-      <c r="F73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" customFormat="1" spans="5:5">
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" customFormat="1" ht="26" customHeight="1" spans="2:5">
-      <c r="B75" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E75" s="15"/>
-    </row>
-    <row r="76" customFormat="1" spans="5:5">
-      <c r="E76" s="15"/>
-    </row>
-    <row r="77" customFormat="1" spans="1:6">
-      <c r="A77">
-        <v>2</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C77" t="s">
-        <v>24</v>
-      </c>
-      <c r="D77" t="s">
-        <v>92</v>
-      </c>
-      <c r="E77" s="15">
-        <v>45747</v>
-      </c>
-      <c r="F77" t="s">
-        <v>10</v>
-      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="1" spans="5:5">
+      <c r="E75" s="14"/>
+    </row>
+    <row r="76" customFormat="1" ht="26" customHeight="1" spans="2:5">
+      <c r="B76" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E76" s="14"/>
+    </row>
+    <row r="77" customFormat="1" spans="5:5">
+      <c r="E77" s="14"/>
     </row>
     <row r="78" customFormat="1" spans="1:6">
       <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="14">
+        <v>45747</v>
+      </c>
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" customFormat="1" spans="1:6">
+      <c r="A79">
         <v>141</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B79" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" t="s">
         <v>8</v>
       </c>
-      <c r="D78" t="s">
-        <v>96</v>
-      </c>
-      <c r="E78" s="15">
+      <c r="D79" t="s">
+        <v>98</v>
+      </c>
+      <c r="E79" s="14">
         <v>45748</v>
       </c>
-      <c r="F78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" ht="35" customHeight="1" spans="2:2">
-      <c r="B80" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82">
-        <v>226</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C82" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="F79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" ht="35" customHeight="1" spans="2:2">
+      <c r="B81" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="E82" s="15">
-        <v>45733</v>
-      </c>
-      <c r="F82" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83">
-        <v>101</v>
+        <v>226</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>100</v>
@@ -2840,8 +2846,8 @@
       <c r="D83" t="s">
         <v>101</v>
       </c>
-      <c r="E83" s="15">
-        <v>45839</v>
+      <c r="E83" s="14">
+        <v>45733</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -2849,7 +2855,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>102</v>
@@ -2860,8 +2866,8 @@
       <c r="D84" t="s">
         <v>103</v>
       </c>
-      <c r="E84" s="15">
-        <v>45856</v>
+      <c r="E84" s="14">
+        <v>45839</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -2869,7 +2875,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>104</v>
@@ -2880,8 +2886,8 @@
       <c r="D85" t="s">
         <v>105</v>
       </c>
-      <c r="E85" s="15">
-        <v>45858</v>
+      <c r="E85" s="14">
+        <v>45856</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
@@ -2889,7 +2895,7 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>106</v>
@@ -2900,114 +2906,114 @@
       <c r="D86" t="s">
         <v>107</v>
       </c>
-      <c r="E86" s="15">
+      <c r="E86" s="14">
+        <v>45858</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
+        <v>144</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>109</v>
+      </c>
+      <c r="E87" s="14">
         <v>45871</v>
       </c>
-      <c r="F86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" ht="39" customHeight="1" spans="2:2">
-      <c r="B88" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90">
-        <v>704</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C90" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" ht="39" customHeight="1" spans="2:2">
+      <c r="B89" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="E90" s="15">
-        <v>45757</v>
-      </c>
-      <c r="F90" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C91" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D91" t="s">
         <v>112</v>
       </c>
-      <c r="E91" s="15">
+      <c r="E91" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>33</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" t="s">
+        <v>114</v>
+      </c>
+      <c r="E92" s="14">
         <v>45759</v>
       </c>
-      <c r="F91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" ht="32" customHeight="1" spans="2:2">
-      <c r="B93" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="95" ht="30" customHeight="1" spans="1:6">
-      <c r="A95">
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" ht="32" customHeight="1" spans="2:2">
+      <c r="B94" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" ht="30" customHeight="1" spans="1:6">
+      <c r="A96">
         <v>34</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B96" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C96" t="s">
         <v>24</v>
       </c>
-      <c r="D95" t="s">
-        <v>115</v>
-      </c>
-      <c r="E95" s="15">
+      <c r="D96" t="s">
+        <v>117</v>
+      </c>
+      <c r="E96" s="14">
         <v>45773</v>
       </c>
-      <c r="F95" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" ht="29" customHeight="1" spans="2:2">
-      <c r="B97" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99">
-        <v>226</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" t="s">
-        <v>117</v>
-      </c>
-      <c r="E99" s="15">
-        <v>45774</v>
-      </c>
-      <c r="F99" t="s">
-        <v>10</v>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" ht="29" customHeight="1" spans="2:2">
+      <c r="B98" s="12" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
@@ -3015,8 +3021,8 @@
       <c r="D100" t="s">
         <v>119</v>
       </c>
-      <c r="E100" s="15">
-        <v>45782</v>
+      <c r="E100" s="14">
+        <v>45774</v>
       </c>
       <c r="F100" t="s">
         <v>10</v>
@@ -3024,7 +3030,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>120</v>
@@ -3035,53 +3041,53 @@
       <c r="D101" t="s">
         <v>121</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E101" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>112</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" s="14">
         <v>45842</v>
       </c>
-      <c r="F101" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2">
-      <c r="B103" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105">
-        <v>100</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C105" t="s">
-        <v>8</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="F102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="E105" s="15">
-        <v>45784</v>
-      </c>
-      <c r="F105" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C106" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D106" t="s">
         <v>126</v>
       </c>
-      <c r="E106" s="15">
-        <v>45785</v>
+      <c r="E106" s="14">
+        <v>45784</v>
       </c>
       <c r="F106" t="s">
         <v>10</v>
@@ -3089,7 +3095,7 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>127</v>
@@ -3100,66 +3106,66 @@
       <c r="D107" t="s">
         <v>128</v>
       </c>
-      <c r="E107" s="15">
+      <c r="E107" s="14">
+        <v>45785</v>
+      </c>
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C108" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" t="s">
+        <v>130</v>
+      </c>
+      <c r="E108" s="14">
         <v>45850</v>
       </c>
-      <c r="F107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" ht="27" customHeight="1" spans="2:2">
-      <c r="B109" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111">
+      <c r="F108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" ht="27" customHeight="1" spans="2:2">
+      <c r="B110" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112">
         <v>235</v>
       </c>
-      <c r="B111" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="B112" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C112" t="s">
         <v>24</v>
       </c>
-      <c r="D111" t="s">
-        <v>131</v>
-      </c>
-      <c r="E111" s="15">
+      <c r="D112" t="s">
+        <v>133</v>
+      </c>
+      <c r="E112" s="14">
         <v>45786</v>
       </c>
-      <c r="F111" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" ht="24" customHeight="1" spans="2:2">
-      <c r="B113" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115">
-        <v>133</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C115" t="s">
-        <v>24</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="F112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" ht="24" customHeight="1" spans="2:2">
+      <c r="B114" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="E115" s="15">
-        <v>45791</v>
-      </c>
-      <c r="F115" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>135</v>
@@ -3170,8 +3176,8 @@
       <c r="D116" t="s">
         <v>136</v>
       </c>
-      <c r="E116" s="15">
-        <v>45806</v>
+      <c r="E116" s="14">
+        <v>45791</v>
       </c>
       <c r="F116" t="s">
         <v>10</v>
@@ -3179,7 +3185,7 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>137</v>
@@ -3190,8 +3196,8 @@
       <c r="D117" t="s">
         <v>138</v>
       </c>
-      <c r="E117" s="15">
-        <v>45807</v>
+      <c r="E117" s="14">
+        <v>45806</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
@@ -3199,19 +3205,19 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C118" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D118" t="s">
         <v>140</v>
       </c>
-      <c r="E118" s="15">
-        <v>45833</v>
+      <c r="E118" s="14">
+        <v>45807</v>
       </c>
       <c r="F118" t="s">
         <v>10</v>
@@ -3219,52 +3225,52 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>141</v>
       </c>
       <c r="C119" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D119" t="s">
         <v>142</v>
       </c>
-      <c r="E119" s="15">
+      <c r="E119" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F119" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120">
+        <v>994</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C120" t="s">
+        <v>24</v>
+      </c>
+      <c r="D120" t="s">
+        <v>144</v>
+      </c>
+      <c r="E120" s="14">
         <v>45834</v>
       </c>
-      <c r="F119" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" ht="29" customHeight="1" spans="2:2">
-      <c r="B121" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123">
-        <v>106</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C123" t="s">
-        <v>24</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="F120" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" ht="29" customHeight="1" spans="2:2">
+      <c r="B122" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="E123" s="15">
-        <v>45782</v>
-      </c>
-      <c r="F123" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>146</v>
@@ -3275,77 +3281,97 @@
       <c r="D124" t="s">
         <v>147</v>
       </c>
-      <c r="E124" s="15">
+      <c r="E124" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F124" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
+        <v>207</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C125" t="s">
+        <v>24</v>
+      </c>
+      <c r="D125" t="s">
+        <v>149</v>
+      </c>
+      <c r="E125" s="14">
         <v>45817</v>
       </c>
-      <c r="F124" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" ht="35" customHeight="1" spans="2:2">
-      <c r="B126" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128">
+      <c r="F125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" ht="35" customHeight="1" spans="2:2">
+      <c r="B127" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129">
         <v>127</v>
       </c>
-      <c r="B128" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C128" t="s">
-        <v>150</v>
-      </c>
-      <c r="D128" t="s">
+      <c r="B129" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E128" s="15">
+      <c r="C129" t="s">
+        <v>152</v>
+      </c>
+      <c r="D129" t="s">
+        <v>153</v>
+      </c>
+      <c r="E129" s="14">
         <v>45831</v>
       </c>
-      <c r="F128" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" ht="41" customHeight="1" spans="1:2">
-      <c r="A134" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B134" s="19">
+      <c r="F129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" ht="41" customHeight="1" spans="1:2">
+      <c r="A135" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B135" s="19">
         <f>COUNT(A:A)</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="136" ht="30" customHeight="1" spans="1:2">
-      <c r="A136" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B136" s="21">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="137" ht="30" customHeight="1" spans="1:2">
+      <c r="A137" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B137" s="21">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="137" ht="40" customHeight="1" spans="1:2">
-      <c r="A137" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="B137" s="23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" ht="40" customHeight="1" spans="1:2">
+      <c r="A138" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B138" s="23">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>34</v>
       </c>
     </row>
-    <row r="138" ht="36" customHeight="1" spans="1:2">
-      <c r="A138" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B138" s="25">
+    <row r="139" ht="36" customHeight="1" spans="1:2">
+      <c r="A139" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B139" s="25">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B128" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B129" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
904. Fruit Into Baskets (Sliding window)
</commit_message>
<xml_diff>
--- a/50  days challenge/DSA_trackerSheet.xlsx
+++ b/50  days challenge/DSA_trackerSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="159">
   <si>
     <t>Q No.</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Arrays,sliding window,hashmap</t>
+  </si>
+  <si>
+    <t>Fruit Into Baskets</t>
   </si>
   <si>
     <t>Heap (Basics)</t>
@@ -1873,10 +1876,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2571,303 +2574,303 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" ht="31" customHeight="1" spans="2:2">
-      <c r="B52" s="12" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>904</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>3066</v>
-      </c>
-      <c r="B54" s="5" t="s">
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="14">
+        <v>45873</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" ht="31" customHeight="1" spans="2:2">
+      <c r="B53" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="C54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="14">
-        <v>45701</v>
-      </c>
-      <c r="F54" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
+        <v>3066</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="14">
+        <v>45701</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
         <v>2099</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B56" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" t="s">
         <v>8</v>
       </c>
-      <c r="D55" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" s="14">
+      <c r="D56" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="14">
         <v>45836</v>
       </c>
-      <c r="F55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" ht="38" customHeight="1" spans="2:2">
-      <c r="B57" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
-        <v>20</v>
-      </c>
-      <c r="B59" s="5" t="s">
+      <c r="F56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" ht="38" customHeight="1" spans="2:2">
+      <c r="B58" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="C59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" t="s">
-        <v>79</v>
-      </c>
-      <c r="E59" s="14">
-        <v>45719</v>
-      </c>
-      <c r="F59" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
+        <v>20</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" s="14">
+        <v>45719</v>
+      </c>
+      <c r="F60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
         <v>155</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B61" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" t="s">
         <v>24</v>
       </c>
-      <c r="D60" t="s">
-        <v>81</v>
-      </c>
-      <c r="E60" s="14">
+      <c r="D61" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="14">
         <v>45731</v>
       </c>
-      <c r="F60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" ht="40" customHeight="1" spans="2:2">
-      <c r="B62" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64">
+      <c r="F61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" ht="40" customHeight="1" spans="2:2">
+      <c r="B63" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
         <v>739</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B65" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" t="s">
         <v>24</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65" s="14">
+        <v>45732</v>
+      </c>
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" s="1" customFormat="1" spans="1:6">
+      <c r="A66" s="15">
         <v>84</v>
       </c>
-      <c r="E64" s="14">
-        <v>45732</v>
-      </c>
-      <c r="F64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" s="1" customFormat="1" spans="1:6">
-      <c r="A65" s="15">
-        <v>84</v>
-      </c>
-      <c r="B65" s="5" t="s">
+      <c r="B66" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E65" s="16">
+      <c r="E66" s="16">
         <v>45745</v>
       </c>
-      <c r="F65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" ht="34" customHeight="1" spans="2:2">
-      <c r="B67" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="69" ht="18" spans="1:6">
-      <c r="A69">
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" ht="34" customHeight="1" spans="2:2">
+      <c r="B68" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" ht="18" spans="1:6">
+      <c r="A70">
         <v>225</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B70" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C70" t="s">
         <v>8</v>
       </c>
-      <c r="D69" t="s">
-        <v>89</v>
-      </c>
-      <c r="E69" s="14">
+      <c r="D70" t="s">
+        <v>90</v>
+      </c>
+      <c r="E70" s="14">
         <v>45841</v>
       </c>
-      <c r="F69" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B71" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="73" customFormat="1" ht="18" spans="1:6">
-      <c r="A73">
+      <c r="F70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B72" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" ht="18" spans="1:6">
+      <c r="A74">
         <v>206</v>
       </c>
-      <c r="B73" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C73" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="B74" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="E73" s="14">
-        <v>45746</v>
-      </c>
-      <c r="F73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" customFormat="1" spans="1:6">
-      <c r="A74">
-        <v>21</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
       </c>
       <c r="D74" t="s">
+        <v>93</v>
+      </c>
+      <c r="E74" s="14">
+        <v>45746</v>
+      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="1" spans="1:6">
+      <c r="A75">
+        <v>21</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E74" s="14">
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>95</v>
+      </c>
+      <c r="E75" s="14">
         <v>45747</v>
       </c>
-      <c r="F74" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" customFormat="1" spans="5:5">
-      <c r="E75" s="14"/>
-    </row>
-    <row r="76" customFormat="1" ht="26" customHeight="1" spans="2:5">
-      <c r="B76" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" customFormat="1" spans="5:5">
       <c r="E76" s="14"/>
     </row>
-    <row r="77" customFormat="1" spans="5:5">
+    <row r="77" customFormat="1" ht="26" customHeight="1" spans="2:5">
+      <c r="B77" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="E77" s="14"/>
     </row>
-    <row r="78" customFormat="1" spans="1:6">
-      <c r="A78">
-        <v>2</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C78" t="s">
-        <v>24</v>
-      </c>
-      <c r="D78" t="s">
-        <v>94</v>
-      </c>
-      <c r="E78" s="14">
-        <v>45747</v>
-      </c>
-      <c r="F78" t="s">
-        <v>10</v>
-      </c>
+    <row r="78" customFormat="1" spans="5:5">
+      <c r="E78" s="14"/>
     </row>
     <row r="79" customFormat="1" spans="1:6">
       <c r="A79">
-        <v>141</v>
+        <v>2</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C79" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" t="s">
+        <v>95</v>
+      </c>
+      <c r="E79" s="14">
+        <v>45747</v>
+      </c>
+      <c r="F79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" customFormat="1" spans="1:6">
+      <c r="A80">
+        <v>141</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" t="s">
         <v>8</v>
       </c>
-      <c r="D79" t="s">
-        <v>98</v>
-      </c>
-      <c r="E79" s="14">
+      <c r="D80" t="s">
+        <v>99</v>
+      </c>
+      <c r="E80" s="14">
         <v>45748</v>
       </c>
-      <c r="F79" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" ht="35" customHeight="1" spans="2:2">
-      <c r="B81" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83">
-        <v>226</v>
-      </c>
-      <c r="B83" s="5" t="s">
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" ht="35" customHeight="1" spans="2:2">
+      <c r="B82" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="C83" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" t="s">
-        <v>101</v>
-      </c>
-      <c r="E83" s="14">
-        <v>45733</v>
-      </c>
-      <c r="F83" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
+        <v>226</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
       </c>
       <c r="D84" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E84" s="14">
-        <v>45839</v>
+        <v>45733</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -2875,19 +2878,19 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E85" s="14">
-        <v>45856</v>
+        <v>45839</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
@@ -2895,19 +2898,19 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E86" s="14">
-        <v>45858</v>
+        <v>45856</v>
       </c>
       <c r="F86" t="s">
         <v>10</v>
@@ -2915,134 +2918,134 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
         <v>8</v>
       </c>
       <c r="D87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87" s="14">
+        <v>45858</v>
+      </c>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <v>144</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E87" s="14">
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>110</v>
+      </c>
+      <c r="E88" s="14">
         <v>45871</v>
       </c>
-      <c r="F87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" ht="39" customHeight="1" spans="2:2">
-      <c r="B89" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91">
-        <v>704</v>
-      </c>
-      <c r="B91" s="5" t="s">
+      <c r="F88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" ht="39" customHeight="1" spans="2:2">
+      <c r="B90" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="C91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" t="s">
-        <v>112</v>
-      </c>
-      <c r="E91" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F91" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92">
+        <v>704</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>113</v>
+      </c>
+      <c r="E92" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
         <v>33</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B93" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C93" t="s">
         <v>24</v>
       </c>
-      <c r="D92" t="s">
-        <v>114</v>
-      </c>
-      <c r="E92" s="14">
+      <c r="D93" t="s">
+        <v>115</v>
+      </c>
+      <c r="E93" s="14">
         <v>45759</v>
       </c>
-      <c r="F92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" ht="32" customHeight="1" spans="2:2">
-      <c r="B94" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="96" ht="30" customHeight="1" spans="1:6">
-      <c r="A96">
+      <c r="F93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" ht="32" customHeight="1" spans="2:2">
+      <c r="B95" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" ht="30" customHeight="1" spans="1:6">
+      <c r="A97">
         <v>34</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="B97" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97" t="s">
         <v>24</v>
       </c>
-      <c r="D96" t="s">
-        <v>117</v>
-      </c>
-      <c r="E96" s="14">
+      <c r="D97" t="s">
+        <v>118</v>
+      </c>
+      <c r="E97" s="14">
         <v>45773</v>
       </c>
-      <c r="F96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" ht="29" customHeight="1" spans="2:2">
-      <c r="B98" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100">
-        <v>226</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="F97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" ht="29" customHeight="1" spans="2:2">
+      <c r="B99" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="E100" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F100" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E101" s="14">
-        <v>45782</v>
+        <v>45774</v>
       </c>
       <c r="F101" t="s">
         <v>10</v>
@@ -3050,64 +3053,64 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
       </c>
       <c r="D102" t="s">
+        <v>122</v>
+      </c>
+      <c r="E102" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>112</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E102" s="14">
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>124</v>
+      </c>
+      <c r="E103" s="14">
         <v>45842</v>
       </c>
-      <c r="F102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2">
-      <c r="B104" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106">
-        <v>100</v>
-      </c>
-      <c r="B106" s="5" t="s">
+      <c r="F103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="C106" t="s">
-        <v>8</v>
-      </c>
-      <c r="D106" t="s">
-        <v>126</v>
-      </c>
-      <c r="E106" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F106" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
         <v>127</v>
       </c>
-      <c r="C107" t="s">
-        <v>24</v>
-      </c>
-      <c r="D107" t="s">
-        <v>128</v>
-      </c>
       <c r="E107" s="14">
-        <v>45785</v>
+        <v>45784</v>
       </c>
       <c r="F107" t="s">
         <v>10</v>
@@ -3115,89 +3118,89 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
         <v>24</v>
       </c>
       <c r="D108" t="s">
+        <v>129</v>
+      </c>
+      <c r="E108" s="14">
+        <v>45785</v>
+      </c>
+      <c r="F108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E108" s="14">
+      <c r="C109" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" t="s">
+        <v>131</v>
+      </c>
+      <c r="E109" s="14">
         <v>45850</v>
       </c>
-      <c r="F108" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" ht="27" customHeight="1" spans="2:2">
-      <c r="B110" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112">
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" ht="27" customHeight="1" spans="2:2">
+      <c r="B111" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
         <v>235</v>
       </c>
-      <c r="B112" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C112" t="s">
+      <c r="B113" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C113" t="s">
         <v>24</v>
       </c>
-      <c r="D112" t="s">
-        <v>133</v>
-      </c>
-      <c r="E112" s="14">
+      <c r="D113" t="s">
+        <v>134</v>
+      </c>
+      <c r="E113" s="14">
         <v>45786</v>
       </c>
-      <c r="F112" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" ht="24" customHeight="1" spans="2:2">
-      <c r="B114" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116">
-        <v>133</v>
-      </c>
-      <c r="B116" s="5" t="s">
+      <c r="F113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" ht="24" customHeight="1" spans="2:2">
+      <c r="B115" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C116" t="s">
-        <v>24</v>
-      </c>
-      <c r="D116" t="s">
-        <v>136</v>
-      </c>
-      <c r="E116" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F116" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C117" t="s">
         <v>24</v>
       </c>
       <c r="D117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E117" s="14">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
@@ -3205,19 +3208,19 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C118" t="s">
         <v>24</v>
       </c>
       <c r="D118" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E118" s="14">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F118" t="s">
         <v>10</v>
@@ -3225,19 +3228,19 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B119" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C119" t="s">
+        <v>24</v>
+      </c>
+      <c r="D119" t="s">
         <v>141</v>
       </c>
-      <c r="C119" t="s">
-        <v>8</v>
-      </c>
-      <c r="D119" t="s">
-        <v>142</v>
-      </c>
       <c r="E119" s="14">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
@@ -3245,133 +3248,153 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120">
+        <v>733</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" t="s">
+        <v>143</v>
+      </c>
+      <c r="E120" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F120" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
         <v>994</v>
       </c>
-      <c r="B120" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="B121" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C121" t="s">
         <v>24</v>
       </c>
-      <c r="D120" t="s">
-        <v>144</v>
-      </c>
-      <c r="E120" s="14">
+      <c r="D121" t="s">
+        <v>145</v>
+      </c>
+      <c r="E121" s="14">
         <v>45834</v>
       </c>
-      <c r="F120" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" ht="29" customHeight="1" spans="2:2">
-      <c r="B122" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124">
-        <v>106</v>
-      </c>
-      <c r="B124" s="5" t="s">
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" ht="29" customHeight="1" spans="2:2">
+      <c r="B123" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="C124" t="s">
-        <v>24</v>
-      </c>
-      <c r="D124" t="s">
-        <v>147</v>
-      </c>
-      <c r="E124" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F124" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C125" t="s">
         <v>24</v>
       </c>
       <c r="D125" t="s">
+        <v>148</v>
+      </c>
+      <c r="E125" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
+        <v>207</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E125" s="14">
+      <c r="C126" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" t="s">
+        <v>150</v>
+      </c>
+      <c r="E126" s="14">
         <v>45817</v>
       </c>
-      <c r="F125" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" ht="35" customHeight="1" spans="2:2">
-      <c r="B127" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129">
+      <c r="F126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" ht="35" customHeight="1" spans="2:2">
+      <c r="B128" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130">
         <v>127</v>
       </c>
-      <c r="B129" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="B130" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D129" t="s">
+      <c r="C130" t="s">
         <v>153</v>
       </c>
-      <c r="E129" s="14">
+      <c r="D130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E130" s="14">
         <v>45831</v>
       </c>
-      <c r="F129" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="135" ht="41" customHeight="1" spans="1:2">
-      <c r="A135" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B135" s="19">
+      <c r="F130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" ht="41" customHeight="1" spans="1:2">
+      <c r="A136" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B136" s="19">
         <f>COUNT(A:A)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="137" ht="30" customHeight="1" spans="1:2">
-      <c r="A137" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B137" s="21">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="138" ht="30" customHeight="1" spans="1:2">
+      <c r="A138" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B138" s="21">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>29</v>
       </c>
     </row>
-    <row r="138" ht="40" customHeight="1" spans="1:2">
-      <c r="A138" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="B138" s="23">
+    <row r="139" ht="40" customHeight="1" spans="1:2">
+      <c r="A139" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B139" s="23">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="139" ht="36" customHeight="1" spans="1:2">
-      <c r="A139" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="B139" s="25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="140" ht="36" customHeight="1" spans="1:2">
+      <c r="A140" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B140" s="25">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B129" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B130" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>